<commit_message>
Add total price calculator,stable
</commit_message>
<xml_diff>
--- a/Lists.xlsx
+++ b/Lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drpre\OneDrive\Desktop\IntroductionToEngineering\AutomaticTrolleySystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A39BE52-720F-40C5-B2C6-1FF34EABF786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2298909-76D2-4868-94BD-560F8DAAC63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7360" xr2:uid="{EC67142D-A09E-46C1-9E7F-E222AEAAD774}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">product name </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>S.No</t>
   </si>
@@ -70,6 +67,18 @@
   </si>
   <si>
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdiOsWQMywLXJV4NX9jYJwzXsW3mjDjmJDOE5EAsFzcN3N30g/viewform?usp=sf_link</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>HandWash</t>
+  </si>
+  <si>
+    <t>Pencil</t>
+  </si>
+  <si>
+    <t>https://vithelpcenter.vit.ac.in/vitcc-help-center/</t>
   </si>
 </sst>
 </file>
@@ -425,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907C3A60-826A-4BC6-A5D1-F65DD0DD9EAB}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,13 +448,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -453,7 +462,7 @@
         <v>45495266138445</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -461,7 +470,7 @@
         <v>8902080404094</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -472,7 +481,7 @@
         <v>8901725013721</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -483,7 +492,7 @@
         <v>8901207038389</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>95</v>
@@ -494,7 +503,7 @@
         <v>8906073772658</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>40</v>
@@ -505,7 +514,7 @@
         <v>8901277012319</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>175</v>
@@ -516,7 +525,7 @@
         <v>8901860633662</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -527,7 +536,7 @@
         <v>8901248101103</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>42</v>
@@ -538,7 +547,7 @@
         <v>8904355401883</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>80</v>
@@ -549,7 +558,7 @@
         <v>8901030937521</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>220</v>
@@ -560,7 +569,7 @@
         <v>8710103905882</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>400</v>
@@ -568,7 +577,24 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>